<commit_message>
Add download data use as CSV
</commit_message>
<xml_diff>
--- a/public/DataUseUploadTemplate.xlsx
+++ b/public/DataUseUploadTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Massimo.Cianfroccapaconsulting.com/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F1B380-842E-9F4C-B42C-FBFA66F54147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAD09C-6A12-8244-B9A5-386BB819C452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{975AA5D9-6C1B-4AA7-819A-A36C7438C5F1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
     <sheet name="Guidance" sheetId="4" r:id="rId2"/>
     <sheet name="Data Uses Template" sheetId="6" r:id="rId3"/>
-    <sheet name="Lookups" sheetId="3" r:id="rId4"/>
+    <sheet name="Lookups" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_ftnref1" localSheetId="1">Guidance!$C$66</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="174">
   <si>
     <t>Health Data Research Innovation Gateway data use register</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Guidance for Completing the Data Uses Template</t>
   </si>
   <si>
-    <t xml:space="preserve">* Please note, that 6 mandatory fields (Organisation Name, Project Title, Lay Summary, Latest Approval Date and Dataset(s) Name, TRE or other specified location) must be completed for each data use, before your data use register can be successfully uploaded. These mandatory fields have been highlighted in grey and by an asterisk. </t>
-  </si>
-  <si>
     <t>5 Safes</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Safe People</t>
   </si>
   <si>
-    <t>Organisation Name*</t>
-  </si>
-  <si>
     <t>The name of the legal entity that signs the contract to access the data</t>
   </si>
   <si>
@@ -96,12 +90,6 @@
   </si>
   <si>
     <t xml:space="preserve">Select relevant sector from list </t>
-  </si>
-  <si>
-    <t>Applicant Names</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name of the Principle Investigator, as well as any other individuals that have been authorised to use the data. If they are on the Gateway, please provide their profile URL </t>
   </si>
   <si>
     <t>Free text in the format First Name, Surname. Separate each applicant with a comma
@@ -129,9 +117,6 @@
     <t>Accreditation status of principal applicant is unknown</t>
   </si>
   <si>
-    <t>Sub-Licence Arrangements (if any)?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Identifies whether there are any permissions for the applicant to share the data beyond the named parties.  e.g., NHS Digital may approve a data release to the ONS, who then makes decisions about access to accredited researchers undertaking approved projects in their own trusted research environment. </t>
   </si>
   <si>
@@ -144,16 +129,7 @@
     <t>Project ID</t>
   </si>
   <si>
-    <t>A unique identifier for the project that is preferably an industry used standard, such as IRAS ID. However for non research projects, a unique reference number created by the data custodian on receipt of the application is sufficient</t>
-  </si>
-  <si>
-    <t>Project Title*</t>
-  </si>
-  <si>
     <t>The title of the project/research study/request that the applicant is investigating through the use of health data</t>
-  </si>
-  <si>
-    <t>Lay Summary*</t>
   </si>
   <si>
     <r>
@@ -175,9 +151,6 @@
     <t>Free text with a maximum of 300 words</t>
   </si>
   <si>
-    <t>Public Benefit Statement</t>
-  </si>
-  <si>
     <t>A description in plain English of the anticipated outcomes, or impact of project on the general public</t>
   </si>
   <si>
@@ -190,51 +163,29 @@
     <t>Select most relevant category from list</t>
   </si>
   <si>
-    <t xml:space="preserve">Technical Summary </t>
-  </si>
-  <si>
     <t xml:space="preserve">A summary of the proposed research, in a manner that is suitable for a specialist reader </t>
   </si>
   <si>
-    <t xml:space="preserve">Other Approval Committees </t>
-  </si>
-  <si>
     <t>Reference to other decision-making bodies that the project has already been authorised by</t>
   </si>
   <si>
-    <t xml:space="preserve">Project Start Date </t>
-  </si>
-  <si>
     <t xml:space="preserve">The date the project is scheduled to start or actual start date </t>
   </si>
   <si>
     <t>ISO 8601 format (YYYY-MM-DD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Project End Date </t>
-  </si>
-  <si>
     <t>The date the project is scheduled to finish or actual end date</t>
   </si>
   <si>
-    <t>Latest Approval Date*</t>
-  </si>
-  <si>
     <t>The last date the data access request for this project was approved by a data custodian</t>
   </si>
   <si>
     <t>Safe Data</t>
-  </si>
-  <si>
-    <t>Dataset(s) Name*</t>
   </si>
   <si>
     <t>The name of the dataset(s) being accessed. If a dataset is on the Gateway, please input the name as it appears on the Gateway or provide the  dataset's URL. 
 Multiple datasets should be separated by a comma.</t>
-  </si>
-  <si>
-    <t>Free text. Input Dataset name as it appears on the Gateway
-Orp rovide the Gateway dataset URL. Separate each dataset by a comma</t>
   </si>
   <si>
     <t>Data Sensitivity Level</t>
@@ -298,9 +249,6 @@
     <t>Not applicable as confidential patient information is not being shared</t>
   </si>
   <si>
-    <t>National Data Opt-out applied?</t>
-  </si>
-  <si>
     <t>Specifies whether the preference for people to opt-out of their confidential patient information being used for secondary use has been applied to the data prior to release</t>
   </si>
   <si>
@@ -353,25 +301,12 @@
     <t>Free text. Separate each field by a comma</t>
   </si>
   <si>
-    <t>Release/Access Date</t>
-  </si>
-  <si>
     <t>The date the data access was granted and active research started</t>
   </si>
   <si>
     <t>Safe Setting</t>
   </si>
   <si>
-    <t>Trusted Research Environment (TRE) or other specified location(s) where data use will take place*</t>
-  </si>
-  <si>
-    <t>These are highly secure spaces for researchers to access sensitive data (also known as Data Safe Havens). A list of available TREs will be provided. If another location has been used, select 'Other'</t>
-  </si>
-  <si>
-    <t>Select one TRE from list.
-If data is not being accessed in a TRE, select 'Other'</t>
-  </si>
-  <si>
     <t>How has data been processed to enhance privacy?</t>
   </si>
   <si>
@@ -379,9 +314,6 @@
   </si>
   <si>
     <t>Safe Outputs</t>
-  </si>
-  <si>
-    <t>Link to Research Outputs</t>
   </si>
   <si>
     <t>A URL link to any academic or non-academic research outputs, as they become available, including code used</t>
@@ -394,35 +326,9 @@
     <t>Safe Project</t>
   </si>
   <si>
-    <t>Applicant Name(s)</t>
-  </si>
-  <si>
     <t>Funders/ Sponsors</t>
   </si>
   <si>
-    <t xml:space="preserve">Project Start Date
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project End Date
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dataset(s) Name*
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Request Frequency
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Release/Access Date
-</t>
-  </si>
-  <si>
-    <t>TRE or any other specified location*</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sub-Licence Arrangements </t>
   </si>
   <si>
@@ -435,58 +341,37 @@
     <t>Academic Institute</t>
   </si>
   <si>
-    <t>NHS Digital</t>
-  </si>
-  <si>
     <t>Efficacy &amp; Mechanism Evaluation</t>
   </si>
   <si>
     <t>CQC Registered Health or/and Social Care provider</t>
   </si>
   <si>
-    <t>Northern Ireland Honest Broker Service (NI HBS)</t>
-  </si>
-  <si>
     <t>Health Services &amp; Delivery</t>
   </si>
   <si>
     <t>Independent Sector Organisation</t>
   </si>
   <si>
-    <t>ONS Secure Research Service (SRS)</t>
-  </si>
-  <si>
     <t>Health Technology Assessment</t>
   </si>
   <si>
     <t>Government Agency (Health and Adult Social Care)</t>
   </si>
   <si>
-    <t>SAIL Databank</t>
-  </si>
-  <si>
     <t>Public Health Research</t>
   </si>
   <si>
     <t>Commercial</t>
   </si>
   <si>
-    <t>Scottish National Safe Haven (SNSH)</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
     <t>Local authority</t>
   </si>
   <si>
-    <t>Secure e-Research Platform (SeRP)</t>
-  </si>
-  <si>
     <t>Government Agency (Other)</t>
-  </si>
-  <si>
-    <t>Organisation Sector</t>
   </si>
   <si>
     <t>To be a full accredited researcher, individuals must have an undergraduate degree (or higher) including a significant proportion of maths or statistics or be able to demonstrate at least three years quantitative research experience. Successful completion of a Safe Researcher training course is also required as part of the accreditation process. Full accredited researcher status is valid for five years.
@@ -501,9 +386,6 @@
   </si>
   <si>
     <t>For linked datasets, specify how the linkage will take place</t>
-  </si>
-  <si>
-    <t>Specifies whether applicant intends for the datasets to be linked with any additional datasets. Relevant information on the organisations undertaking linkages and how the linkage will take place mjust also be disclosed. As well as, a summary of the risks/mitigations to be considered</t>
   </si>
   <si>
     <t>If confidential information is being disclosed , the organisations holding this data (both the organisation disclosing the information and the recipient organisation) must also have a lawful basis to hold and use this information, and if applicable, have a condition to hold and use special categories of confidential information, and be fair and transparent about how they hold and use this data.
@@ -515,12 +397,6 @@
     <t>Processing of personal data revealing racial or ethnic origin, political opinions, religious or philosophical beliefs, or trade union membership, and the processing of genetic data, biometric data for the purpose of uniquely identifying a natural person, data concerning health or data concerning a natural person's sex life or sexual orientation shall be prohibited. This does not apply if one of the following applies.</t>
   </si>
   <si>
-    <t>DEA Accredited Researcher?</t>
-  </si>
-  <si>
-    <t>Depending on the type of data you are requesting, you might be required to become an accredited researcher. Most access to data in the Secure Research Service (SRS) will be by researchers accredited under the Digital Economy Act 2017 (DEA). This specifies the accreditation status of the principle applicant/researcher, as defined by the ONS Research Code of Practice and Accreditation criteria</t>
-  </si>
-  <si>
     <t>Legal basis for provision of data under Article 6</t>
   </si>
   <si>
@@ -586,10 +462,139 @@
     <t>(f) processing is necessary for the purposes of the legitimate interests pursued by the controller or by a third party, except where such interests are overridden by the interests or fundamental rights and freedoms of the data subject which require protection of personal data, in particular where the data subject is a child.</t>
   </si>
   <si>
-    <t>Technical Summary</t>
-  </si>
-  <si>
-    <t>Other Approval Committees</t>
+    <t>Organisation name*</t>
+  </si>
+  <si>
+    <t>Organisation sector</t>
+  </si>
+  <si>
+    <t>Applicant names</t>
+  </si>
+  <si>
+    <t>DEA accredited researcher?</t>
+  </si>
+  <si>
+    <t>Sub-licence arrangements (if any)?</t>
+  </si>
+  <si>
+    <t>Project title*</t>
+  </si>
+  <si>
+    <t>Lay summary*</t>
+  </si>
+  <si>
+    <t>Public benefit statement</t>
+  </si>
+  <si>
+    <t>Request category type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical summary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other approval committees </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project start date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project end date </t>
+  </si>
+  <si>
+    <t>Latest approval date*</t>
+  </si>
+  <si>
+    <t>Dataset(s) name*</t>
+  </si>
+  <si>
+    <t>Data sensitivity level</t>
+  </si>
+  <si>
+    <t>National data opt-out applied?</t>
+  </si>
+  <si>
+    <t>Request frequency</t>
+  </si>
+  <si>
+    <t>Release/Access date</t>
+  </si>
+  <si>
+    <t>Access type</t>
+  </si>
+  <si>
+    <t>Determines whether the data will be accessed within a Trusted Research Environment (TRE) or via the traditional data release model</t>
+  </si>
+  <si>
+    <t>Select one access type from list.</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Data will be accessed within a Trusted Research Environment</t>
+  </si>
+  <si>
+    <t>Data will be accessed via the release of data extract</t>
+  </si>
+  <si>
+    <t>Access Type</t>
+  </si>
+  <si>
+    <t>Access type*</t>
+  </si>
+  <si>
+    <t>Link to research outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release/Access date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request frequency
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataset(s) name*
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project end date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project start date
+</t>
+  </si>
+  <si>
+    <t>Public benefit statement*</t>
+  </si>
+  <si>
+    <t>Applicant name(s)</t>
+  </si>
+  <si>
+    <t>Depending on the type of data you are requesting, you might be required to become an accredited researcher. Most access to data in the Secure Research Service (SRS) will be by researchers accredited under the Digital Economy Act 2017 (DEA). This specifies the accreditation status of the principal applicant/researcher, as defined by the ONS Research Code of Practice and Accreditation criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the Principal Investigator, as well as any other individuals that have been authorised to use the data. If they are on the Gateway, please provide their profile URL </t>
+  </si>
+  <si>
+    <t>A unique identifier for the project that is preferably an industry used standard, such as IRAS ID. However for non-research projects, a unique reference number created by the data custodian on receipt of the application is sufficient</t>
+  </si>
+  <si>
+    <t>Free text. Input Dataset name as it appears on the Gateway
+Or provide the Gateway dataset URL. Separate each dataset by a comma</t>
+  </si>
+  <si>
+    <t>Specifies whether applicant intends for the datasets to be linked with any additional datasets. Relevant information on the organisations undertaking linkages and how the linkage will take place must also be disclosed. As well as, a summary of the risks/mitigations to be considered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Please note, there are 7 recommended minimum fields (organisation name, project title, lay summary, public benefit statement, latest approval date, dataset(s) name and access type) that should be completed for each data use, before uploading your register onto the Gateway. These recommended minimum fields have been highlighted in grey and by an asterisk.   </t>
+  </si>
+  <si>
+    <t>Technical summary</t>
+  </si>
+  <si>
+    <t>Other approval committees</t>
   </si>
 </sst>
 </file>
@@ -738,7 +743,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,42 +784,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -998,7 +967,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1121,77 +1090,68 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1224,8 +1184,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5013960</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1240,8 +1200,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="220980" y="434340"/>
-          <a:ext cx="9364980" cy="2628900"/>
+          <a:off x="220980" y="426720"/>
+          <a:ext cx="9349740" cy="2667000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1282,13 +1242,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>In line with the recommendations set out in the Alliance Green Paper, the Gateway Data Use register is based on the Five Safes framework.  This is to to enable ease of understanding and aggregation of registers. </a:t>
+            <a:t>In line with the recommendations set out in the Alliance Green Paper, the Gateway data use register is based on the Five Safes framework.  This is to to enable ease of understanding and aggregation of registers. </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Custodians listing datasets on the gateway are requested to provide as much data use information about approved data uses. The information will be published as part of the Gateway Data Use Register and show up as a related resource of the relevant dataset listings.</a:t>
+            <a:t>Custodians listing datasets on the Gateway are requested to provide as much information about approved data uses as possible. The information will be published as part of the Gateway Data Use Register and show up as a related resource of the relevant dataset listings.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1297,7 +1257,55 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Please note, that only the 5 mandatory fields (Organisation Name, Project Title, Lay Summary, Latest Approval Date and Dataset(s) Name, TRE o) must be completed for each data use, before it can be successfully uploaded. These mandatory fields have been highlighted in grey and by an asterisk.  Whilst this is the minimum, Custodians are encouraged to complete as many data fields as their internal data use register allows. </a:t>
+            <a:t>Please note, there are 7 recommended minimum fields (organisation name, project title, lay summary, public</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> benefit statement, l</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>atest approval date,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> d</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>ataset(s) name</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> and a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>ccess</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> type</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>) that should be completed for each data use, before uploading</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> your register onto the Gateway.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t> These recommended minimum fields have been highlighted in grey and by an asterisk.  Whilst this is the minimum, data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> c</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>ustodians are encouraged to complete as many data fields as their internal data use register allows. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1607,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20B1AB5-8A76-4FB7-8CF9-042426A646B4}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1622,10 +1630,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" customHeight="1">
       <c r="A1" s="38"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="63"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" ht="12.5" customHeight="1">
       <c r="A2" s="38"/>
@@ -1645,29 +1653,29 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="40" t="s">
+    <row r="8" spans="1:3">
+      <c r="B8" s="40" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="9" customHeight="1">
-      <c r="B8" s="41"/>
-    </row>
-    <row r="9" spans="1:3" ht="16">
-      <c r="B9" s="42" t="s">
+    <row r="9" spans="1:3" ht="9" customHeight="1">
+      <c r="B9" s="41"/>
+    </row>
+    <row r="10" spans="1:3" ht="16">
+      <c r="B10" s="42" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="43"/>
+    <row r="12" spans="1:3">
+      <c r="B12" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B7" location="Guidance!A1" display="Read Guidance" xr:uid="{18031A18-751E-4EC1-B0BD-1F19EAA187C3}"/>
-    <hyperlink ref="B9" location="'Data Uses Template'!A1" display="Complete Template" xr:uid="{A8764B9D-F70C-4572-9755-201D75D42D6C}"/>
+    <hyperlink ref="B8" location="Guidance!A1" display="Read Guidance" xr:uid="{18031A18-751E-4EC1-B0BD-1F19EAA187C3}"/>
+    <hyperlink ref="B10" location="'Data Uses Template'!A1" display="Complete Template" xr:uid="{A8764B9D-F70C-4572-9755-201D75D42D6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1680,10 +1688,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E71"/>
+  <dimension ref="B1:E73"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1696,19 +1704,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="21" customHeight="1">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="2:5" ht="42" customHeight="1">
-      <c r="B2" s="68" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
+      <c r="B2" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="39"/>
@@ -1717,743 +1725,769 @@
     </row>
     <row r="4" spans="2:5" ht="17">
       <c r="B4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="E4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="31" t="s">
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="68" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="66" t="s">
+      <c r="C5" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="E5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="37" t="s">
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="68"/>
+      <c r="C6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="D6" s="36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="66"/>
-      <c r="C6" s="48" t="s">
+      <c r="E6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="36" t="s">
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="68"/>
+      <c r="C7" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="36" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="66"/>
-      <c r="C7" s="48" t="s">
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="48">
+      <c r="B8" s="68"/>
+      <c r="C8" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="32">
+      <c r="B9" s="68"/>
+      <c r="C9" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="68"/>
+      <c r="C10" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="47.5" customHeight="1">
+      <c r="B11" s="68"/>
+      <c r="C11" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="96">
+      <c r="B12" s="68"/>
+      <c r="C12" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="60"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="68"/>
+      <c r="C13" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="60"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="68"/>
+      <c r="C14" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="61"/>
+    </row>
+    <row r="15" spans="2:5" ht="32">
+      <c r="B15" s="68"/>
+      <c r="C15" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="32">
+      <c r="B16" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="66"/>
+      <c r="C17" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="32">
+      <c r="B18" s="66"/>
+      <c r="C18" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="66"/>
+      <c r="C19" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="66"/>
+      <c r="C20" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="48">
-      <c r="B8" s="66"/>
-      <c r="C8" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="66"/>
+      <c r="C21" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="66"/>
+      <c r="C22" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="32">
-      <c r="B9" s="66"/>
-      <c r="C9" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="36" t="s">
+    <row r="23" spans="2:5">
+      <c r="B23" s="66"/>
+      <c r="C23" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="66"/>
+      <c r="C24" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="66"/>
+      <c r="C25" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="32">
+      <c r="B26" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="14.5" customHeight="1">
+      <c r="B27" s="68"/>
+      <c r="C27" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="68"/>
+      <c r="C28" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="60"/>
+    </row>
+    <row r="29" spans="2:5" ht="48">
+      <c r="B29" s="68"/>
+      <c r="C29" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="60"/>
+    </row>
+    <row r="30" spans="2:5" ht="32">
+      <c r="B30" s="68"/>
+      <c r="C30" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="61"/>
+    </row>
+    <row r="31" spans="2:5" ht="33.5" customHeight="1">
+      <c r="B31" s="68"/>
+      <c r="C31" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="26">
+      <c r="B32" s="68"/>
+      <c r="C32" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="60"/>
+    </row>
+    <row r="33" spans="2:5" ht="29" customHeight="1">
+      <c r="B33" s="68"/>
+      <c r="C33" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="60"/>
+    </row>
+    <row r="34" spans="2:5" ht="27" customHeight="1">
+      <c r="B34" s="68"/>
+      <c r="C34" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="60"/>
+    </row>
+    <row r="35" spans="2:5" ht="27" customHeight="1">
+      <c r="B35" s="68"/>
+      <c r="C35" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="60"/>
+    </row>
+    <row r="36" spans="2:5" ht="39">
+      <c r="B36" s="68"/>
+      <c r="C36" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="60"/>
+    </row>
+    <row r="37" spans="2:5" ht="65">
+      <c r="B37" s="68"/>
+      <c r="C37" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="60"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="68"/>
+      <c r="C38" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="60"/>
+    </row>
+    <row r="39" spans="2:5" ht="48">
+      <c r="B39" s="68"/>
+      <c r="C39" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="52">
+      <c r="B40" s="68"/>
+      <c r="C40" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="60"/>
+    </row>
+    <row r="41" spans="2:5" ht="91">
+      <c r="B41" s="68"/>
+      <c r="C41" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="60"/>
+    </row>
+    <row r="42" spans="2:5" ht="39">
+      <c r="B42" s="68"/>
+      <c r="C42" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="60"/>
+    </row>
+    <row r="43" spans="2:5" ht="91">
+      <c r="B43" s="68"/>
+      <c r="C43" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="60"/>
+    </row>
+    <row r="44" spans="2:5" ht="26">
+      <c r="B44" s="68"/>
+      <c r="C44" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="60"/>
+    </row>
+    <row r="45" spans="2:5" ht="26">
+      <c r="B45" s="68"/>
+      <c r="C45" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="60"/>
+    </row>
+    <row r="46" spans="2:5" ht="65">
+      <c r="B46" s="68"/>
+      <c r="C46" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="60"/>
+    </row>
+    <row r="47" spans="2:5" ht="91">
+      <c r="B47" s="68"/>
+      <c r="C47" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="60"/>
+    </row>
+    <row r="48" spans="2:5" ht="91">
+      <c r="B48" s="68"/>
+      <c r="C48" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="60"/>
+    </row>
+    <row r="49" spans="2:5" ht="78">
+      <c r="B49" s="68"/>
+      <c r="C49" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E49" s="60"/>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="68"/>
+      <c r="C50" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50" s="61"/>
+    </row>
+    <row r="51" spans="2:5" ht="72" customHeight="1">
+      <c r="B51" s="68"/>
+      <c r="C51" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" s="59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="68"/>
+      <c r="C52" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52" s="60"/>
+    </row>
+    <row r="53" spans="2:5" ht="29" customHeight="1">
+      <c r="B53" s="68"/>
+      <c r="C53" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="60"/>
+    </row>
+    <row r="54" spans="2:5" ht="29" customHeight="1">
+      <c r="B54" s="68"/>
+      <c r="C54" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="60"/>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="68"/>
+      <c r="C55" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E55" s="61"/>
+    </row>
+    <row r="56" spans="2:5" ht="14.5" customHeight="1">
+      <c r="B56" s="68"/>
+      <c r="C56" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" s="59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="68"/>
+      <c r="C57" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" s="60"/>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="68"/>
+      <c r="C58" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" s="60"/>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="68"/>
+      <c r="C59" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59" s="61"/>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" s="68"/>
+      <c r="C60" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" s="68"/>
+      <c r="C61" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" s="60"/>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="68"/>
+      <c r="C62" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" s="60"/>
+    </row>
+    <row r="63" spans="2:5" ht="32">
+      <c r="B63" s="68"/>
+      <c r="C63" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" s="68"/>
+      <c r="C64" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="68"/>
+      <c r="C65" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="66"/>
-      <c r="C10" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="47.5" customHeight="1">
-      <c r="B11" s="66"/>
-      <c r="C11" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E11" s="69" t="s">
+      <c r="E66" s="62" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="96">
-      <c r="B12" s="66"/>
-      <c r="C12" s="57" t="s">
+    <row r="67" spans="2:5">
+      <c r="B67" s="66"/>
+      <c r="C67" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E67" s="63"/>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="66"/>
+      <c r="C68" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" s="64"/>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="67"/>
+      <c r="C69" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E12" s="70"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="66"/>
-      <c r="C13" s="57" t="s">
+      <c r="D69" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="32">
+      <c r="B70" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="70"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="66"/>
-      <c r="C14" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="71"/>
-    </row>
-    <row r="15" spans="2:5" ht="32">
-      <c r="B15" s="66"/>
-      <c r="C15" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="32">
-      <c r="B16" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="67"/>
-      <c r="C17" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="32">
-      <c r="B18" s="67"/>
-      <c r="C18" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="67"/>
-      <c r="C19" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="67"/>
-      <c r="C20" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="67"/>
-      <c r="C21" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="67"/>
-      <c r="C22" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="67"/>
-      <c r="C23" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="67"/>
-      <c r="C24" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="67"/>
-      <c r="C25" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="32">
-      <c r="B26" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="14.5" customHeight="1">
-      <c r="B27" s="66"/>
-      <c r="C27" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="69" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="66"/>
-      <c r="C28" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="70"/>
-    </row>
-    <row r="29" spans="2:5" ht="48">
-      <c r="B29" s="66"/>
-      <c r="C29" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="70"/>
-    </row>
-    <row r="30" spans="2:5" ht="32">
-      <c r="B30" s="66"/>
-      <c r="C30" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="71"/>
-    </row>
-    <row r="31" spans="2:5" ht="33.5" customHeight="1">
-      <c r="B31" s="66"/>
-      <c r="C31" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E31" s="69" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="26">
-      <c r="B32" s="66"/>
-      <c r="C32" s="62" t="s">
-        <v>164</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E32" s="70"/>
-    </row>
-    <row r="33" spans="2:5" ht="29" customHeight="1">
-      <c r="B33" s="66"/>
-      <c r="C33" s="62" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E33" s="70"/>
-    </row>
-    <row r="34" spans="2:5" ht="27" customHeight="1">
-      <c r="B34" s="66"/>
-      <c r="C34" s="62" t="s">
-        <v>166</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E34" s="70"/>
-    </row>
-    <row r="35" spans="2:5" ht="27" customHeight="1">
-      <c r="B35" s="66"/>
-      <c r="C35" s="62" t="s">
-        <v>167</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E35" s="70"/>
-    </row>
-    <row r="36" spans="2:5" ht="39">
-      <c r="B36" s="66"/>
-      <c r="C36" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="70"/>
-    </row>
-    <row r="37" spans="2:5" ht="65">
-      <c r="B37" s="66"/>
-      <c r="C37" s="62" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E37" s="70"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="66"/>
-      <c r="C38" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="70"/>
-    </row>
-    <row r="39" spans="2:5" ht="48">
-      <c r="B39" s="66"/>
-      <c r="C39" s="56" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" s="70" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="52">
-      <c r="B40" s="66"/>
-      <c r="C40" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E40" s="70"/>
-    </row>
-    <row r="41" spans="2:5" ht="91">
-      <c r="B41" s="66"/>
-      <c r="C41" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E41" s="70"/>
-    </row>
-    <row r="42" spans="2:5" ht="39">
-      <c r="B42" s="66"/>
-      <c r="C42" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="70"/>
-    </row>
-    <row r="43" spans="2:5" ht="91">
-      <c r="B43" s="66"/>
-      <c r="C43" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="70"/>
-    </row>
-    <row r="44" spans="2:5" ht="26">
-      <c r="B44" s="66"/>
-      <c r="C44" s="62" t="s">
+      <c r="C70" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="70"/>
-    </row>
-    <row r="45" spans="2:5" ht="26">
-      <c r="B45" s="66"/>
-      <c r="C45" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="70"/>
-    </row>
-    <row r="46" spans="2:5" ht="65">
-      <c r="B46" s="66"/>
-      <c r="C46" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="70"/>
-    </row>
-    <row r="47" spans="2:5" ht="91">
-      <c r="B47" s="66"/>
-      <c r="C47" s="62" t="s">
-        <v>161</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="70"/>
-    </row>
-    <row r="48" spans="2:5" ht="91">
-      <c r="B48" s="66"/>
-      <c r="C48" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" s="70"/>
-    </row>
-    <row r="49" spans="2:5" ht="91">
-      <c r="B49" s="66"/>
-      <c r="C49" s="62" t="s">
-        <v>163</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E49" s="70"/>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="66"/>
-      <c r="C50" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" s="71"/>
-    </row>
-    <row r="51" spans="2:5" ht="72" customHeight="1">
-      <c r="B51" s="66"/>
-      <c r="C51" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="69" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="66"/>
-      <c r="C52" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="70"/>
-    </row>
-    <row r="53" spans="2:5" ht="29" customHeight="1">
-      <c r="B53" s="66"/>
-      <c r="C53" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="70"/>
-    </row>
-    <row r="54" spans="2:5" ht="29" customHeight="1">
-      <c r="B54" s="66"/>
-      <c r="C54" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E54" s="70"/>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" s="66"/>
-      <c r="C55" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E55" s="71"/>
-    </row>
-    <row r="56" spans="2:5" ht="14.5" customHeight="1">
-      <c r="B56" s="66"/>
-      <c r="C56" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E56" s="69" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="66"/>
-      <c r="C57" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E57" s="70"/>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="66"/>
-      <c r="C58" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E58" s="70"/>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="B59" s="66"/>
-      <c r="C59" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="71"/>
-    </row>
-    <row r="60" spans="2:5">
-      <c r="B60" s="66"/>
-      <c r="C60" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="69" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="B61" s="66"/>
-      <c r="C61" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E61" s="70"/>
-    </row>
-    <row r="62" spans="2:5">
-      <c r="B62" s="66"/>
-      <c r="C62" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E62" s="70"/>
-    </row>
-    <row r="63" spans="2:5" ht="32">
-      <c r="B63" s="66"/>
-      <c r="C63" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5">
-      <c r="B64" s="66"/>
-      <c r="C64" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5">
-      <c r="B65" s="66"/>
-      <c r="C65" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="32">
-      <c r="B66" s="64" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="E66" s="37" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="65"/>
-      <c r="C67" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E67" s="36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="32">
-      <c r="B68" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="C68" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="D69"/>
-    </row>
-    <row r="70" spans="2:5">
-      <c r="D70"/>
-    </row>
-    <row r="71" spans="2:5" ht="19">
-      <c r="B71" s="35"/>
-      <c r="C71" s="5"/>
+    </row>
+    <row r="71" spans="2:5">
       <c r="D71"/>
     </row>
+    <row r="72" spans="2:5">
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="2:5" ht="19">
+      <c r="B73" s="35"/>
+      <c r="C73" s="5"/>
+      <c r="D73"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B5:B15"/>
+    <mergeCell ref="B16:B25"/>
+    <mergeCell ref="B26:B65"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="E56:E59"/>
     <mergeCell ref="E60:E62"/>
     <mergeCell ref="B1:E1"/>
@@ -2462,11 +2496,6 @@
     <mergeCell ref="E51:E55"/>
     <mergeCell ref="E31:E38"/>
     <mergeCell ref="E39:E50"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B5:B15"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="B26:B65"/>
-    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2477,47 +2506,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773C5661-484B-4AB5-AC73-DC8AD2E35A84}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="255.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="255.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5" style="45" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="46" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="79.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="76.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="254.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" style="24" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" style="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="254.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="255.83203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.1640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="254.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="23" customWidth="1"/>
+    <col min="3" max="4" width="13.5" style="24" customWidth="1"/>
+    <col min="5" max="7" width="9.5" style="24" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="13" style="25" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="24" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" style="45" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="45" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" style="46" customWidth="1"/>
+    <col min="19" max="19" width="15.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" style="24" customWidth="1"/>
+    <col min="21" max="22" width="22.6640625" style="24" customWidth="1"/>
+    <col min="23" max="23" width="19" style="24" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="24" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.83203125" style="24" customWidth="1"/>
+    <col min="27" max="27" width="15" style="24" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" style="46" customWidth="1"/>
+    <col min="29" max="29" width="18" style="23" customWidth="1"/>
+    <col min="30" max="30" width="19.1640625" style="26" customWidth="1"/>
+    <col min="31" max="31" width="21.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="17" customFormat="1" ht="22" thickBot="1">
       <c r="B1" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -2527,7 +2553,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="20"/>
       <c r="J1" s="18" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
@@ -2538,7 +2564,7 @@
       <c r="Q1" s="19"/>
       <c r="R1" s="20"/>
       <c r="S1" s="18" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="T1" s="19"/>
       <c r="U1" s="19"/>
@@ -2550,112 +2576,112 @@
       <c r="AA1" s="19"/>
       <c r="AB1" s="19"/>
       <c r="AC1" s="18" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="AD1" s="20"/>
       <c r="AE1" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" s="15" customFormat="1" ht="65" thickBot="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="15" customFormat="1" ht="64">
       <c r="A2" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="N2" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="U2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="32" t="s">
+      <c r="V2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="W2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="Y2" s="32" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="Z2" s="32" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="AA2" s="32" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="AB2" s="32" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="AC2" s="14" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="AE2" s="27" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576" xr:uid="{8EB9EB01-5558-4105-B0D8-072792F17C1F}"/>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You have not entered a valid date" prompt="Input date in the format_x000a_YYYY-MM-DD" sqref="AB6:AB1048576 P6:R1048576" xr:uid="{865CB1AE-04BE-4F15-A2A7-6B0029F8DBA7}">
+    <dataValidation operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K1048576" xr:uid="{8EB9EB01-5558-4105-B0D8-072792F17C1F}"/>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You have not entered a valid date" prompt="Input date in the format_x000a_YYYY-MM-DD" sqref="AB3:AB1048576 P3:R1048576" xr:uid="{865CB1AE-04BE-4F15-A2A7-6B0029F8DBA7}">
       <formula1>36526</formula1>
       <formula2>55153</formula2>
     </dataValidation>
@@ -2663,72 +2689,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9D53DD6E-976E-46B1-B2C3-4C986057E79C}">
           <x14:formula1>
             <xm:f>Lookups!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H20308</xm:sqref>
+          <xm:sqref>H3:H20308</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82375C37-9F27-41F0-B89A-8BE61F25F375}">
           <x14:formula1>
             <xm:f>Lookups!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I6:I20308</xm:sqref>
+          <xm:sqref>I3:I20308</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{80815C9E-E914-4DFF-9793-1A245D48E2BC}">
           <x14:formula1>
             <xm:f>Lookups!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>T6:T20308</xm:sqref>
+          <xm:sqref>T3:T20308</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A87B30F8-09C5-4E68-BAE3-834302C89407}">
           <x14:formula1>
             <xm:f>Lookups!$H$2:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X6:X20427</xm:sqref>
+          <xm:sqref>X3:X20427</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AAF7F0A-ED76-48EF-80A7-D58E0D3201EB}">
           <x14:formula1>
             <xm:f>Lookups!$J$2:$J$8</xm:f>
           </x14:formula1>
-          <xm:sqref>AC6:AC20308</xm:sqref>
+          <xm:sqref>AC20274:AC20308</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6A412C1-3DC6-4E1E-B832-3631B4D3664E}">
           <x14:formula1>
             <xm:f>Lookups!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M20941</xm:sqref>
+          <xm:sqref>M3:M20941</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C61A458-24E0-4927-92E6-CD319CABF41E}">
           <x14:formula1>
             <xm:f>Lookups!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D10421</xm:sqref>
+          <xm:sqref>D3:D10421</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD5CE6AA-455D-4A48-8E23-96E415AF85F0}">
           <x14:formula1>
             <xm:f>Lookups!$F$2:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>W6:W20427</xm:sqref>
+          <xm:sqref>W3:W20427</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA9B1993-2762-42CD-96AF-654A5DC152B3}">
           <x14:formula1>
             <xm:f>Lookups!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Y6:Y20427</xm:sqref>
+          <xm:sqref>Y3:Y20427</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{375B382A-F51E-49E1-995F-4ABA7D067F1D}">
           <x14:formula1>
             <xm:f>Lookups!$D$2:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>U6:U20427</xm:sqref>
+          <xm:sqref>U3:U20427</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4CA7B91B-AE5F-461E-BC61-25B90C94D828}">
           <x14:formula1>
             <xm:f>Lookups!$E$2:$E$12</xm:f>
           </x14:formula1>
-          <xm:sqref>V6:V20427</xm:sqref>
+          <xm:sqref>V3:V20427</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{91317689-55DB-4675-B0F3-BC8486BC081E}">
+          <x14:formula1>
+            <xm:f>Lookups!$J$2:$J$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AC3:AC20273</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2740,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A21CB1F-7D69-4C22-91CF-207A2396B9E2}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2759,233 +2791,218 @@
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" ht="33" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>150</v>
+        <v>89</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>111</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="K2" s="44" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="128">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="224">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="7" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="I4" s="7"/>
-      <c r="J4" t="s">
-        <v>128</v>
-      </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="96">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="7" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="G5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" t="s">
-        <v>131</v>
-      </c>
       <c r="K5" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="256">
       <c r="A6" s="1" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="7" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="8"/>
       <c r="I6" s="1"/>
-      <c r="J6" t="s">
-        <v>134</v>
-      </c>
       <c r="K6" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="80">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="7" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="8"/>
       <c r="I7" s="1"/>
-      <c r="J7" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="8" spans="1:11" ht="176">
       <c r="A8" s="1" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="7" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="9" spans="1:11" ht="176">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -2997,7 +3014,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -3009,7 +3026,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -3018,7 +3035,7 @@
     <row r="12" spans="1:11" ht="224">
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:11">

</xml_diff>